<commit_message>
IBPDI Real Estate CDM update Version : 2.0
</commit_message>
<xml_diff>
--- a/Documentation/Change Logs/IBPDI V2.0 change log.xlsx
+++ b/Documentation/Change Logs/IBPDI V2.0 change log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuathiele/Desktop/IBPDI/_CDM/CDM_V2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuathiele/ibpdi git/cdm/Documentation/Change Logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA908329-4417-D24F-8BCE-28621B663B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B96E78-445E-8D44-8235-394BB2AAEF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{518BE735-91D0-994C-801D-4FB1302BB870}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{518BE735-91D0-994C-801D-4FB1302BB870}"/>
   </bookViews>
   <sheets>
     <sheet name="Changes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="101">
   <si>
     <t>Cluster</t>
   </si>
@@ -235,6 +235,111 @@
   </si>
   <si>
     <t>delete (or depricate) stated that not used yet</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>change to CertificateValue (ontology)</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Add pattern https?:\/\/(?:www\.|(?!www))[a-zA-Z0-9][a-zA-Z0-9-]+[a-zA-Z0-9]\.[^\s]{2,}|www\.[a-zA-Z0-9][a-zA-Z0-9-]+[a-zA-Z0-9]\.[^\s]{2,}|https?:\/\/(?:www\.|(?!www))[a-zA-Z0-9]+\.[^\s]{2,}|www\.[a-zA-Z0-9]+\.[^\s]{2,}</t>
+  </si>
+  <si>
+    <t>CertificateUrl</t>
+  </si>
+  <si>
+    <t>IssuingDate</t>
+  </si>
+  <si>
+    <t>correct comment [{"dataType":"dateTime"}]</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>change name to IbpdiProject (ontology)</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>change name to IbpdiCategory (ontology)</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>change name to IbpdiGroup (ontology)</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>BookingCurrency</t>
+  </si>
+  <si>
+    <t>Add pattern [^&lt;&gt;\[\]\{\}\|\\\/\(\)°"&amp;=\+§\^~:;\$%!\?\0-\cZ]+$</t>
+  </si>
+  <si>
+    <t>PortfolioAndAssetManagement</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>ReportingDate</t>
+  </si>
+  <si>
+    <t>ReportingCycle</t>
+  </si>
+  <si>
+    <t>PortfolioStrategy</t>
+  </si>
+  <si>
+    <t>StrategyObjectiveUnit</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>StrategyObjectiveUnitSteering</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>IndividualAccountPortfolio</t>
+  </si>
+  <si>
+    <t>PortfolioId</t>
+  </si>
+  <si>
+    <t>change fk name</t>
+  </si>
+  <si>
+    <t>PropertyManagement</t>
+  </si>
+  <si>
+    <t>Dunning</t>
+  </si>
+  <si>
+    <t>RentalPayment</t>
   </si>
 </sst>
 </file>
@@ -602,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83EE764-28B3-F84B-BF7B-E75215E0A336}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1331,6 +1436,295 @@
         <v>29</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{A83EE764-28B3-F84B-BF7B-E75215E0A336}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>